<commit_message>
Added: Explainations of addressing PCF8574 boards.
</commit_message>
<xml_diff>
--- a/Hardware listing.xlsx
+++ b/Hardware listing.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\favier\Documents\GitHub\ControlPanel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Commun\Informatique\Projets\Control Panel BO\Dépôt GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A330AB2-57E3-41AE-B45C-2FFC8EF89005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nomenclature FR" sheetId="2" r:id="rId1"/>
     <sheet name="Nomenclature EN" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Racailloux</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +39,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Papier + Cartouche + Laque brillante</t>
         </r>
@@ -49,12 +50,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Racailloux</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Papier + Cartouche + Laque brillante</t>
         </r>
@@ -123,12 +124,6 @@
     <t>Bouton poussoir métal illuminé Rouge 16mm</t>
   </si>
   <si>
-    <t>Vis M2 x8mm</t>
-  </si>
-  <si>
-    <t>Vis M4 x12mm</t>
-  </si>
-  <si>
     <t>Antidérapants</t>
   </si>
   <si>
@@ -213,12 +208,6 @@
     <t>black PLA filament</t>
   </si>
   <si>
-    <t>M2 screw x8mm</t>
-  </si>
-  <si>
-    <t>M4 screw x12mm</t>
-  </si>
-  <si>
     <t>Sticker</t>
   </si>
   <si>
@@ -247,12 +236,24 @@
   </si>
   <si>
     <t>Total price</t>
+  </si>
+  <si>
+    <t>M3 screw x8mm</t>
+  </si>
+  <si>
+    <t>M3 screw x12mm</t>
+  </si>
+  <si>
+    <t>Vis M3 x8mm</t>
+  </si>
+  <si>
+    <t>Vis M3 x12mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -289,7 +290,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -513,30 +514,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:F28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:F28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Produits"/>
-    <tableColumn id="2" name="Référence"/>
-    <tableColumn id="3" name="Prix Unitaire" dataDxfId="8"/>
-    <tableColumn id="4" name="Quantité" dataDxfId="7"/>
-    <tableColumn id="6" name="Ports" dataDxfId="6"/>
-    <tableColumn id="5" name="Prix Total" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Produits"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Référence"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prix Unitaire" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quantité" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ports" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Prix Total" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:F28" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau13" displayName="Tableau13" ref="A1:F28" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F28" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Protduct"/>
-    <tableColumn id="2" name="Reference"/>
-    <tableColumn id="3" name="Unit price" dataDxfId="3"/>
-    <tableColumn id="4" name="Quantity" dataDxfId="2"/>
-    <tableColumn id="6" name="Shipping" dataDxfId="1"/>
-    <tableColumn id="5" name="Total price" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Protduct"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reference"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Unit price" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Shipping" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Total price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -838,11 +839,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -864,16 +865,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -900,7 +901,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1114,7 +1115,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -1135,7 +1136,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -1162,7 +1163,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -1184,10 +1185,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="8">
         <f>33.99/120</f>
@@ -1208,10 +1209,10 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="9">
         <v>25.45</v>
@@ -1226,7 +1227,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1248,7 +1249,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1273,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="8">
         <f>10/5</f>
@@ -1289,10 +1290,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" s="8">
         <f>23.99</f>
@@ -1308,10 +1309,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="8">
         <f>11.5</f>
@@ -1327,10 +1328,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="8">
         <f>6.29/30</f>
@@ -1349,7 +1350,7 @@
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
       <c r="E29" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F29" s="12">
         <f>SUM(F2:F28)</f>
@@ -1360,22 +1361,22 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B4:B8" r:id="rId8" display="AliExpress"/>
-    <hyperlink ref="B21:B22" r:id="rId9" display="Aliexpress"/>
-    <hyperlink ref="B18" r:id="rId10"/>
-    <hyperlink ref="B23" r:id="rId11"/>
-    <hyperlink ref="B20" r:id="rId12"/>
-    <hyperlink ref="B26" r:id="rId13"/>
-    <hyperlink ref="B24" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B25" r:id="rId16"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B4:B8" r:id="rId8" display="AliExpress" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B21:B22" r:id="rId9" display="Aliexpress" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B25" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
@@ -1387,11 +1388,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1407,22 +1408,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,7 +1450,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1471,7 +1472,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1492,7 +1493,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1513,7 +1514,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1534,7 +1535,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -1555,7 +1556,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -1598,7 +1599,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1641,7 +1642,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -1663,7 +1664,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -1684,7 +1685,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -1711,7 +1712,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -1733,10 +1734,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="8">
         <f>33.99/120</f>
@@ -1757,10 +1758,10 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="9">
         <v>25.45</v>
@@ -1775,7 +1776,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1797,7 +1798,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1819,10 +1820,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="8">
         <f>10/5</f>
@@ -1838,10 +1839,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" s="8">
         <f>23.99</f>
@@ -1857,10 +1858,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="8">
         <f>11.5</f>
@@ -1876,10 +1877,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="8">
         <f>6.29/30</f>
@@ -1898,7 +1899,7 @@
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
       <c r="E29" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F29" s="12">
         <f>SUM(F2:F28)</f>
@@ -1909,22 +1910,22 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B4:B8" r:id="rId8" display="AliExpress"/>
-    <hyperlink ref="B21:B22" r:id="rId9" display="Aliexpress"/>
-    <hyperlink ref="B18" r:id="rId10"/>
-    <hyperlink ref="B23" r:id="rId11"/>
-    <hyperlink ref="B20" r:id="rId12"/>
-    <hyperlink ref="B26" r:id="rId13"/>
-    <hyperlink ref="B24" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B25" r:id="rId16"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B4:B8" r:id="rId8" display="AliExpress" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B21:B22" r:id="rId9" display="Aliexpress" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B23" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="B25" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
Changed: Update instructions and hardware.
</commit_message>
<xml_diff>
--- a/Hardware listing.xlsx
+++ b/Hardware listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Commun\Informatique\Projets\Control Panel BO\Dépôt GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A330AB2-57E3-41AE-B45C-2FFC8EF89005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C60C06B-5B54-4A13-9065-7F82663C1F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,13 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -133,9 +140,6 @@
     <t>Fil 22AWG</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>SOVB3D</t>
   </si>
   <si>
@@ -248,6 +252,9 @@
   </si>
   <si>
     <t>Vis M3 x12mm</t>
+  </si>
+  <si>
+    <t>TOTAL (est.)</t>
   </si>
 </sst>
 </file>
@@ -843,7 +850,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -865,16 +872,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,7 +908,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1115,7 +1122,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -1136,7 +1143,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -1163,7 +1170,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -1209,10 +1216,10 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="9">
         <v>25.45</v>
@@ -1227,7 +1234,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1249,7 +1256,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1290,7 +1297,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>17</v>
@@ -1309,7 +1316,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>17</v>
@@ -1350,7 +1357,7 @@
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
       <c r="E29" s="11" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="F29" s="12">
         <f>SUM(F2:F28)</f>
@@ -1392,7 +1399,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A22"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1408,22 +1415,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,7 +1457,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1472,7 +1479,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1493,7 +1500,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1514,7 +1521,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1535,7 +1542,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -1556,7 +1563,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -1599,7 +1606,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1642,7 +1649,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -1664,7 +1671,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -1685,7 +1692,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -1712,7 +1719,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -1734,7 +1741,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1758,10 +1765,10 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="9">
         <v>25.45</v>
@@ -1776,7 +1783,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1798,7 +1805,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1820,7 +1827,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
@@ -1839,7 +1846,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>17</v>
@@ -1858,7 +1865,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>17</v>
@@ -1877,7 +1884,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>17</v>
@@ -1899,7 +1906,7 @@
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
       <c r="E29" s="11" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="F29" s="12">
         <f>SUM(F2:F28)</f>

</xml_diff>